<commit_message>
sofia | test3 | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test3.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7C9E58-BA90-4B9B-A6BE-CFDB41B73879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E5D2F2-2066-4B28-B4D6-2854B682E437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -1719,7 +1719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -3088,8 +3088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3473,7 +3473,7 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="D22" s="13">
-        <v>51.5</v>
+        <v>111.9</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>194</v>
@@ -4023,7 +4023,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4102,7 +4102,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
sofia | test3 | bug fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test3.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E5D2F2-2066-4B28-B4D6-2854B682E437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D68F4BD-1A89-4360-BF9D-26A80A35F9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1206,7 +1206,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1285,7 +1285,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:F19"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -3089,7 +3089,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D53" sqref="D2:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3762,7 +3762,7 @@
         <v>0.9</v>
       </c>
       <c r="D39" s="13">
-        <v>10.199999999999999</v>
+        <v>1.8</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>194</v>
@@ -3813,7 +3813,7 @@
         <v>0.9</v>
       </c>
       <c r="D42" s="13">
-        <v>10.3</v>
+        <v>0.4</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>194</v>
@@ -4102,7 +4102,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>